<commit_message>
Changed 54.173.199.137 to localhost
</commit_message>
<xml_diff>
--- a/CandyStoreAutomation/CandyStoreTestData.xlsx
+++ b/CandyStoreAutomation/CandyStoreTestData.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">CandyCount</t>
   </si>
   <si>
-    <t xml:space="preserve">http://54.173.199.137:8080/CandyStore-0.0.3/candyorderREST/getOrder/</t>
+    <t xml:space="preserve">http://localhost:8080/CandyStore/candyorderREST/getOrder/</t>
   </si>
   <si>
     <t xml:space="preserve">Sku</t>
@@ -336,12 +336,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,11 +526,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.7397959183674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,7 +563,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://54.173.199.137:8080/CandyStore"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://localhost:8080/CandyStore/candyorderREST/getOrder/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -588,11 +588,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.7397959183674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,12 +647,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>